<commit_message>
pridane mereni, uz chybi jen jedno 32kove, upraven graf, zprava template(hlavicka+reference)
</commit_message>
<xml_diff>
--- a/trunk/ukol2/src/docs/mereni.xlsx
+++ b/trunk/ukol2/src/docs/mereni.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Infiband</t>
   </si>
@@ -53,6 +53,48 @@
   <si>
     <t>zrychleni proti casu 1</t>
   </si>
+  <si>
+    <t>1-Infiband</t>
+  </si>
+  <si>
+    <t>2-Infiband</t>
+  </si>
+  <si>
+    <t>3-Infiband</t>
+  </si>
+  <si>
+    <t>1-LAN</t>
+  </si>
+  <si>
+    <t>2-LAN</t>
+  </si>
+  <si>
+    <t>3-LAN</t>
+  </si>
+  <si>
+    <t># CPU's</t>
+  </si>
+  <si>
+    <t>zrychleni</t>
+  </si>
+  <si>
+    <t>1 - Infiband</t>
+  </si>
+  <si>
+    <t>2 - Infiband</t>
+  </si>
+  <si>
+    <t>3 - Infiband</t>
+  </si>
+  <si>
+    <t>1 - LAN</t>
+  </si>
+  <si>
+    <t>2 - LAN</t>
+  </si>
+  <si>
+    <t>3 - LAN</t>
+  </si>
 </sst>
 </file>
 
@@ -76,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -133,25 +175,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -171,9 +230,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0599518810148726E-2"/>
-          <c:y val="5.1341131491511538E-2"/>
-          <c:w val="0.69132545931758527"/>
+          <c:x val="0.14895732961194977"/>
+          <c:y val="5.0854263970782188E-2"/>
+          <c:w val="0.69132545931758549"/>
           <c:h val="0.79845833143689404"/>
         </c:manualLayout>
       </c:layout>
@@ -195,10 +254,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$D$4:$D$9</c:f>
+              <c:f>List1!$D$4:$D$10</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -216,6 +275,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>31.39537271544938</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.155783132530118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -267,10 +329,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$F$4:$F$8</c:f>
+              <c:f>List1!$F$4:$F$10</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -285,6 +347,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17.273648275269242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.497285433753035</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.416475209134568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -336,10 +404,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>List1!$H$4:$H$8</c:f>
+              <c:f>List1!$H$4:$H$10</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -354,6 +422,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17.571105319829588</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.326669427606888</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.924484643242359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,7 +511,7 @@
             <c:numRef>
               <c:f>List1!$J$4:$J$8</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:formatCode>0,00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -504,10 +578,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$L$4:$L$8</c:f>
+              <c:f>List1!$L$4:$L$10</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -522,6 +596,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>18.018525444984711</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.894300452727556</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.397430118614665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,10 +653,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>List1!$N$4:$N$8</c:f>
+              <c:f>List1!$N$4:$N$10</c:f>
               <c:numCache>
-                <c:formatCode>Vęeobecný</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -591,37 +671,39 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17.116034202753568</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.764674512465611</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="139077888"/>
-        <c:axId val="139075584"/>
+        <c:axId val="70695168"/>
+        <c:axId val="70709248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139077888"/>
+        <c:axId val="70695168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="Vęeobecný" sourceLinked="1"/>
+        <c:numFmt formatCode="0,00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139075584"/>
+        <c:crossAx val="70709248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139075584"/>
+        <c:axId val="70709248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="Vęeobecný" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139077888"/>
+        <c:crossAx val="70695168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -629,6 +711,580 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="cs-CZ"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Zrychlen</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ"/>
+              <a:t>í</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ" baseline="0"/>
+              <a:t> výpočtu v závislosti na počtu procesorů</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$L$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1-Infiband</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$K$15:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$L$15:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0537940556374421</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1840766897516399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3332349187170962</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.063058035714285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.39537271544938</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.155783132530118</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$M$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2-Infiband</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$K$15:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$M$15:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0083452312964019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2259040895264564</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3212997991617446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.273648275269242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.497285433753035</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.416475209134568</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$N$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3-Infiband</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$K$15:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$N$15:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0634176556395278</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.292531737257443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4897924099804865</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.571105319829588</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.326669427606888</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.924484643242359</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$O$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1-LAN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$K$15:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$O$15:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0286605324879505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2087693835459481</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.365826698006062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.864862548477642</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.713271267752816</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.001305748888917</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$P$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2-LAN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$K$15:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$P$15:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0429638499258753</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2536116284418988</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5339700753104211</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.018525444984711</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.894300452727556</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.397430118614665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$Q$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3-LAN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$K$15:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>Vęeobecný</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$Q$15:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>0,00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.992522462096364</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9526772137092059</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4085363293224038</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.116034202753568</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.764674512465611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="95121408"/>
+        <c:axId val="95086080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="95121408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Počet procesorů</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="Vęeobecný" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95086080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="95086080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Zrychlení výpočtu n-krát</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0,00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95121408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -644,16 +1300,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>396874</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>39687</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>373060</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>103189</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -667,6 +1323,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>412748</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>111126</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graf 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -960,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:R10"/>
+  <dimension ref="B1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -977,54 +1663,54 @@
       </c>
     </row>
     <row r="2" spans="2:18">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="1" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
       <c r="Q2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:18">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="5"/>
       <c r="Q3" t="s">
         <v>8</v>
       </c>
@@ -1033,48 +1719,48 @@
       </c>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>550.38599999999997</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="9">
         <v>562.65800000000002</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="10">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="8">
         <v>562.98699999999997</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="9">
         <v>550.97</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="10">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="8">
         <v>573.27200000000005</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="8">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="9">
         <v>540.66300000000001</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="11">
         <f>1</f>
         <v>1</v>
       </c>
@@ -1086,48 +1772,48 @@
       </c>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>267.98500000000001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <f>C$4/C5</f>
         <v>2.0537940556374421</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="9">
         <v>280.16000000000003</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="10">
         <f>E$4/E5</f>
         <v>2.0083452312964019</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="8">
         <v>272.84199999999998</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <f>G$4/G5</f>
         <v>2.0634176556395278</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="9">
         <v>271.59300000000002</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="10">
         <f>I$4/I5</f>
         <v>2.0286605324879505</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="8">
         <v>280.608</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="8">
         <f>K$4/K5</f>
         <v>2.0429638499258753</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="9">
         <v>271.346</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="11">
         <f>M$4/M5</f>
         <v>1.992522462096364</v>
       </c>
@@ -1139,174 +1825,644 @@
       </c>
     </row>
     <row r="6" spans="2:18">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>131.54300000000001</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <f>C$4/C6</f>
         <v>4.1840766897516399</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="9">
         <v>133.14500000000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="10">
         <f>E$4/E6</f>
         <v>4.2259040895264564</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="8">
         <v>131.155</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="8">
         <f t="shared" ref="H6" si="0">G$4/G6</f>
         <v>4.292531737257443</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="9">
         <v>130.91</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="10">
         <f t="shared" ref="J6" si="1">I$4/I6</f>
         <v>4.2087693835459481</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="8">
         <v>134.773</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="8">
         <f t="shared" ref="L6" si="2">K$4/K6</f>
         <v>4.2536116284418988</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="9">
         <v>136.78399999999999</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="11">
         <f t="shared" ref="N6" si="3">M$4/M6</f>
         <v>3.9526772137092059</v>
       </c>
     </row>
     <row r="7" spans="2:18">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>66.0471</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <f>C$4/C7</f>
         <v>8.3332349187170962</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="9">
         <v>67.616600000000005</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="10">
         <f>E$4/E7</f>
         <v>8.3212997991617446</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <v>66.313400000000001</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="8">
         <f t="shared" ref="H7" si="4">G$4/G7</f>
         <v>8.4897924099804865</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="9">
         <v>65.8596</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="10">
         <f t="shared" ref="J7" si="5">I$4/I7</f>
         <v>8.365826698006062</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="8">
         <v>67.175299999999993</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="8">
         <f t="shared" ref="L7" si="6">K$4/K7</f>
         <v>8.5339700753104211</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="9">
         <v>64.299300000000002</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="11">
         <f t="shared" ref="N7" si="7">M$4/M7</f>
         <v>8.4085363293224038</v>
       </c>
     </row>
     <row r="8" spans="2:18">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>32.256</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <f>C$4/C8</f>
         <v>17.063058035714285</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="9">
         <v>32.5732</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="10">
         <f>E$4/E8</f>
         <v>17.273648275269242</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="8">
         <v>32.040500000000002</v>
       </c>
-      <c r="H8">
-        <f t="shared" ref="H8" si="8">G$4/G8</f>
+      <c r="H8" s="8">
+        <f t="shared" ref="H8:H10" si="8">G$4/G8</f>
         <v>17.571105319829588</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="9">
         <v>32.669699999999999</v>
       </c>
-      <c r="J8" s="3">
-        <f t="shared" ref="J8" si="9">I$4/I8</f>
+      <c r="J8" s="10">
+        <f t="shared" ref="J8:J10" si="9">I$4/I8</f>
         <v>16.864862548477642</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="8">
         <v>31.8157</v>
       </c>
-      <c r="L8">
-        <f t="shared" ref="L8" si="10">K$4/K8</f>
+      <c r="L8" s="8">
+        <f t="shared" ref="L8:L10" si="10">K$4/K8</f>
         <v>18.018525444984711</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="9">
         <v>31.588100000000001</v>
       </c>
-      <c r="N8" s="6">
-        <f t="shared" ref="N8" si="11">M$4/M8</f>
+      <c r="N8" s="11">
+        <f t="shared" ref="N8:N9" si="11">M$4/M8</f>
         <v>17.116034202753568</v>
       </c>
     </row>
     <row r="9" spans="2:18">
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>24</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>17.530799999999999</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <f>C$4/C9</f>
         <v>31.39537271544938</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="3"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
+      <c r="E9" s="9">
+        <v>17.314</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" ref="F9:F10" si="12">E$4/E9</f>
+        <v>32.497285433753035</v>
+      </c>
+      <c r="G9" s="8">
+        <v>15.9366</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="8"/>
+        <v>35.326669427606888</v>
+      </c>
+      <c r="I9" s="9">
+        <v>16.842400000000001</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="9"/>
+        <v>32.713271267752816</v>
+      </c>
+      <c r="K9" s="8">
+        <v>17.427700000000002</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="10"/>
+        <v>32.894300452727556</v>
+      </c>
+      <c r="M9" s="9">
+        <v>16.5014</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="11"/>
+        <v>32.764674512465611</v>
+      </c>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>32</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
+      <c r="C10" s="8">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D10" s="8">
+        <f>C$4/C10</f>
+        <v>33.155783132530118</v>
+      </c>
+      <c r="E10" s="9">
+        <v>15.886900000000001</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="12"/>
+        <v>35.416475209134568</v>
+      </c>
+      <c r="G10" s="8">
+        <v>16.595300000000002</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="8"/>
+        <v>33.924484643242359</v>
+      </c>
+      <c r="I10" s="9">
+        <v>16.695399999999999</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="9"/>
+        <v>33.001305748888917</v>
+      </c>
+      <c r="K10" s="8">
+        <v>16.1953</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" si="10"/>
+        <v>35.397430118614665</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="L13" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13">
+        <v>550.38599999999997</v>
+      </c>
+      <c r="D15" s="13">
+        <v>562.65800000000002</v>
+      </c>
+      <c r="E15" s="13">
+        <v>562.98699999999997</v>
+      </c>
+      <c r="F15" s="13">
+        <v>550.97</v>
+      </c>
+      <c r="G15" s="13">
+        <v>573.27200000000005</v>
+      </c>
+      <c r="H15" s="9">
+        <v>540.66300000000001</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="M15" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="N15" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="O15" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P15" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="Q15" s="9">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13">
+        <v>267.98500000000001</v>
+      </c>
+      <c r="D16" s="13">
+        <v>280.16000000000003</v>
+      </c>
+      <c r="E16" s="13">
+        <v>272.84199999999998</v>
+      </c>
+      <c r="F16" s="13">
+        <v>271.59300000000002</v>
+      </c>
+      <c r="G16" s="13">
+        <v>280.608</v>
+      </c>
+      <c r="H16" s="9">
+        <v>271.346</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="K16" s="2">
+        <v>2</v>
+      </c>
+      <c r="L16" s="13">
+        <f>C$15/C16</f>
+        <v>2.0537940556374421</v>
+      </c>
+      <c r="M16" s="13">
+        <f t="shared" ref="M16:Q16" si="13">D$15/D16</f>
+        <v>2.0083452312964019</v>
+      </c>
+      <c r="N16" s="13">
+        <f t="shared" si="13"/>
+        <v>2.0634176556395278</v>
+      </c>
+      <c r="O16" s="13">
+        <f t="shared" si="13"/>
+        <v>2.0286605324879505</v>
+      </c>
+      <c r="P16" s="13">
+        <f t="shared" si="13"/>
+        <v>2.0429638499258753</v>
+      </c>
+      <c r="Q16" s="9">
+        <f t="shared" si="13"/>
+        <v>1.992522462096364</v>
+      </c>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="2:18">
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="13">
+        <v>131.54300000000001</v>
+      </c>
+      <c r="D17" s="13">
+        <v>133.14500000000001</v>
+      </c>
+      <c r="E17" s="13">
+        <v>131.155</v>
+      </c>
+      <c r="F17" s="13">
+        <v>130.91</v>
+      </c>
+      <c r="G17" s="13">
+        <v>134.773</v>
+      </c>
+      <c r="H17" s="9">
+        <v>136.78399999999999</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="K17" s="2">
+        <v>4</v>
+      </c>
+      <c r="L17" s="13">
+        <f t="shared" ref="L17:L21" si="14">C$15/C17</f>
+        <v>4.1840766897516399</v>
+      </c>
+      <c r="M17" s="13">
+        <f t="shared" ref="M17:M21" si="15">D$15/D17</f>
+        <v>4.2259040895264564</v>
+      </c>
+      <c r="N17" s="13">
+        <f t="shared" ref="N17:N21" si="16">E$15/E17</f>
+        <v>4.292531737257443</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" ref="O17:O21" si="17">F$15/F17</f>
+        <v>4.2087693835459481</v>
+      </c>
+      <c r="P17" s="13">
+        <f t="shared" ref="P17:P21" si="18">G$15/G17</f>
+        <v>4.2536116284418988</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" ref="Q17:Q21" si="19">H$15/H17</f>
+        <v>3.9526772137092059</v>
+      </c>
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="2:18">
+      <c r="B18" s="2">
+        <v>8</v>
+      </c>
+      <c r="C18" s="13">
+        <v>66.0471</v>
+      </c>
+      <c r="D18" s="13">
+        <v>67.616600000000005</v>
+      </c>
+      <c r="E18" s="13">
+        <v>66.313400000000001</v>
+      </c>
+      <c r="F18" s="13">
+        <v>65.8596</v>
+      </c>
+      <c r="G18" s="13">
+        <v>67.175299999999993</v>
+      </c>
+      <c r="H18" s="9">
+        <v>64.299300000000002</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="K18" s="2">
+        <v>8</v>
+      </c>
+      <c r="L18" s="13">
+        <f t="shared" si="14"/>
+        <v>8.3332349187170962</v>
+      </c>
+      <c r="M18" s="13">
+        <f t="shared" si="15"/>
+        <v>8.3212997991617446</v>
+      </c>
+      <c r="N18" s="13">
+        <f t="shared" si="16"/>
+        <v>8.4897924099804865</v>
+      </c>
+      <c r="O18" s="13">
+        <f t="shared" si="17"/>
+        <v>8.365826698006062</v>
+      </c>
+      <c r="P18" s="13">
+        <f t="shared" si="18"/>
+        <v>8.5339700753104211</v>
+      </c>
+      <c r="Q18" s="9">
+        <f t="shared" si="19"/>
+        <v>8.4085363293224038</v>
+      </c>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="2:18">
+      <c r="B19" s="2">
+        <v>16</v>
+      </c>
+      <c r="C19" s="13">
+        <v>32.256</v>
+      </c>
+      <c r="D19" s="13">
+        <v>32.5732</v>
+      </c>
+      <c r="E19" s="13">
+        <v>32.040500000000002</v>
+      </c>
+      <c r="F19" s="13">
+        <v>32.669699999999999</v>
+      </c>
+      <c r="G19" s="13">
+        <v>31.8157</v>
+      </c>
+      <c r="H19" s="9">
+        <v>31.588100000000001</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="K19" s="2">
+        <v>16</v>
+      </c>
+      <c r="L19" s="13">
+        <f t="shared" si="14"/>
+        <v>17.063058035714285</v>
+      </c>
+      <c r="M19" s="13">
+        <f t="shared" si="15"/>
+        <v>17.273648275269242</v>
+      </c>
+      <c r="N19" s="13">
+        <f t="shared" si="16"/>
+        <v>17.571105319829588</v>
+      </c>
+      <c r="O19" s="13">
+        <f t="shared" si="17"/>
+        <v>16.864862548477642</v>
+      </c>
+      <c r="P19" s="13">
+        <f t="shared" si="18"/>
+        <v>18.018525444984711</v>
+      </c>
+      <c r="Q19" s="9">
+        <f t="shared" si="19"/>
+        <v>17.116034202753568</v>
+      </c>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="2:18">
+      <c r="B20" s="2">
+        <v>24</v>
+      </c>
+      <c r="C20" s="13">
+        <v>17.530799999999999</v>
+      </c>
+      <c r="D20" s="13">
+        <v>17.314</v>
+      </c>
+      <c r="E20" s="13">
+        <v>15.9366</v>
+      </c>
+      <c r="F20" s="13">
+        <v>16.842400000000001</v>
+      </c>
+      <c r="G20" s="13">
+        <v>17.427700000000002</v>
+      </c>
+      <c r="H20" s="9">
+        <v>16.5014</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="K20" s="2">
+        <v>24</v>
+      </c>
+      <c r="L20" s="13">
+        <f t="shared" si="14"/>
+        <v>31.39537271544938</v>
+      </c>
+      <c r="M20" s="13">
+        <f t="shared" si="15"/>
+        <v>32.497285433753035</v>
+      </c>
+      <c r="N20" s="13">
+        <f t="shared" si="16"/>
+        <v>35.326669427606888</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="17"/>
+        <v>32.713271267752816</v>
+      </c>
+      <c r="P20" s="13">
+        <f t="shared" si="18"/>
+        <v>32.894300452727556</v>
+      </c>
+      <c r="Q20" s="9">
+        <f t="shared" si="19"/>
+        <v>32.764674512465611</v>
+      </c>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="2:18">
+      <c r="B21" s="2">
+        <v>32</v>
+      </c>
+      <c r="C21" s="13">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D21" s="13">
+        <v>15.886900000000001</v>
+      </c>
+      <c r="E21" s="13">
+        <v>16.595300000000002</v>
+      </c>
+      <c r="F21" s="13">
+        <v>16.695399999999999</v>
+      </c>
+      <c r="G21" s="13">
+        <v>16.1953</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="11"/>
+      <c r="K21" s="2">
+        <v>32</v>
+      </c>
+      <c r="L21" s="13">
+        <f t="shared" si="14"/>
+        <v>33.155783132530118</v>
+      </c>
+      <c r="M21" s="13">
+        <f t="shared" si="15"/>
+        <v>35.416475209134568</v>
+      </c>
+      <c r="N21" s="13">
+        <f t="shared" si="16"/>
+        <v>33.924484643242359</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" si="17"/>
+        <v>33.001305748888917</v>
+      </c>
+      <c r="P21" s="13">
+        <f t="shared" si="18"/>
+        <v>35.397430118614665</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1320,7 +2476,8 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
final 1.0 pls check/correction :)
</commit_message>
<xml_diff>
--- a/trunk/ukol2/src/docs/mereni.xlsx
+++ b/trunk/ukol2/src/docs/mereni.xlsx
@@ -196,6 +196,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -205,12 +211,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -230,9 +230,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14895732961194977"/>
+          <c:x val="0.1489573296119498"/>
           <c:y val="5.0854263970782188E-2"/>
-          <c:w val="0.69132545931758549"/>
+          <c:w val="0.69132545931758571"/>
           <c:h val="0.79845833143689404"/>
         </c:manualLayout>
       </c:layout>
@@ -679,23 +679,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70695168"/>
-        <c:axId val="70709248"/>
+        <c:axId val="91867776"/>
+        <c:axId val="91885952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70695168"/>
+        <c:axId val="91867776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0,00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70709248"/>
+        <c:crossAx val="91885952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70709248"/>
+        <c:axId val="91885952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,20 +703,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="Vęeobecný" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70695168"/>
+        <c:crossAx val="91867776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1200,15 +1199,18 @@
                 <c:pt idx="5">
                   <c:v>32.764674512465611</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.042977624249211</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95121408"/>
-        <c:axId val="95086080"/>
+        <c:axId val="91934080"/>
+        <c:axId val="91940736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95121408"/>
+        <c:axId val="91934080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,12 +1235,12 @@
         </c:title>
         <c:numFmt formatCode="Vęeobecný" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95086080"/>
+        <c:crossAx val="91940736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95086080"/>
+        <c:axId val="91940736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,7 +1266,7 @@
         </c:title>
         <c:numFmt formatCode="0,00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95121408"/>
+        <c:crossAx val="91934080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1290,7 +1292,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1649,7 +1651,7 @@
   <dimension ref="B1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1663,22 +1665,22 @@
       </c>
     </row>
     <row r="2" spans="2:18">
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="5" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
       <c r="Q2" t="s">
         <v>7</v>
       </c>
@@ -1687,30 +1689,30 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="5"/>
+      <c r="N3" s="11"/>
       <c r="Q3" t="s">
         <v>8</v>
       </c>
@@ -1722,45 +1724,45 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>550.38599999999997</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>562.65800000000002</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <v>562.98699999999997</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="6">
         <v>550.97</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="7">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="5">
         <v>573.27200000000005</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="6">
         <v>540.66300000000001</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="8">
         <f>1</f>
         <v>1</v>
       </c>
@@ -1775,45 +1777,45 @@
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>267.98500000000001</v>
       </c>
-      <c r="D5" s="8">
-        <f>C$4/C5</f>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D10" si="0">C$4/C5</f>
         <v>2.0537940556374421</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>280.16000000000003</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <f>E$4/E5</f>
         <v>2.0083452312964019</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>272.84199999999998</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="5">
         <f>G$4/G5</f>
         <v>2.0634176556395278</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="6">
         <v>271.59300000000002</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="7">
         <f>I$4/I5</f>
         <v>2.0286605324879505</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="5">
         <v>280.608</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="5">
         <f>K$4/K5</f>
         <v>2.0429638499258753</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="6">
         <v>271.346</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="8">
         <f>M$4/M5</f>
         <v>1.992522462096364</v>
       </c>
@@ -1828,46 +1830,46 @@
       <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>131.54300000000001</v>
       </c>
-      <c r="D6" s="8">
-        <f>C$4/C6</f>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
         <v>4.1840766897516399</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>133.14500000000001</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <f>E$4/E6</f>
         <v>4.2259040895264564</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <v>131.155</v>
       </c>
-      <c r="H6" s="8">
-        <f t="shared" ref="H6" si="0">G$4/G6</f>
+      <c r="H6" s="5">
+        <f t="shared" ref="H6" si="1">G$4/G6</f>
         <v>4.292531737257443</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="6">
         <v>130.91</v>
       </c>
-      <c r="J6" s="10">
-        <f t="shared" ref="J6" si="1">I$4/I6</f>
+      <c r="J6" s="7">
+        <f t="shared" ref="J6" si="2">I$4/I6</f>
         <v>4.2087693835459481</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="5">
         <v>134.773</v>
       </c>
-      <c r="L6" s="8">
-        <f t="shared" ref="L6" si="2">K$4/K6</f>
+      <c r="L6" s="5">
+        <f t="shared" ref="L6" si="3">K$4/K6</f>
         <v>4.2536116284418988</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="6">
         <v>136.78399999999999</v>
       </c>
-      <c r="N6" s="11">
-        <f t="shared" ref="N6" si="3">M$4/M6</f>
+      <c r="N6" s="8">
+        <f t="shared" ref="N6" si="4">M$4/M6</f>
         <v>3.9526772137092059</v>
       </c>
     </row>
@@ -1875,46 +1877,46 @@
       <c r="B7" s="2">
         <v>8</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <v>66.0471</v>
       </c>
-      <c r="D7" s="8">
-        <f>C$4/C7</f>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
         <v>8.3332349187170962</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>67.616600000000005</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <f>E$4/E7</f>
         <v>8.3212997991617446</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <v>66.313400000000001</v>
       </c>
-      <c r="H7" s="8">
-        <f t="shared" ref="H7" si="4">G$4/G7</f>
+      <c r="H7" s="5">
+        <f t="shared" ref="H7" si="5">G$4/G7</f>
         <v>8.4897924099804865</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="6">
         <v>65.8596</v>
       </c>
-      <c r="J7" s="10">
-        <f t="shared" ref="J7" si="5">I$4/I7</f>
+      <c r="J7" s="7">
+        <f t="shared" ref="J7" si="6">I$4/I7</f>
         <v>8.365826698006062</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="5">
         <v>67.175299999999993</v>
       </c>
-      <c r="L7" s="8">
-        <f t="shared" ref="L7" si="6">K$4/K7</f>
+      <c r="L7" s="5">
+        <f t="shared" ref="L7" si="7">K$4/K7</f>
         <v>8.5339700753104211</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="6">
         <v>64.299300000000002</v>
       </c>
-      <c r="N7" s="11">
-        <f t="shared" ref="N7" si="7">M$4/M7</f>
+      <c r="N7" s="8">
+        <f t="shared" ref="N7" si="8">M$4/M7</f>
         <v>8.4085363293224038</v>
       </c>
     </row>
@@ -1922,46 +1924,46 @@
       <c r="B8" s="2">
         <v>16</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="5">
         <v>32.256</v>
       </c>
-      <c r="D8" s="8">
-        <f>C$4/C8</f>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
         <v>17.063058035714285</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="6">
         <v>32.5732</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <f>E$4/E8</f>
         <v>17.273648275269242</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <v>32.040500000000002</v>
       </c>
-      <c r="H8" s="8">
-        <f t="shared" ref="H8:H10" si="8">G$4/G8</f>
+      <c r="H8" s="5">
+        <f t="shared" ref="H8:H10" si="9">G$4/G8</f>
         <v>17.571105319829588</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="6">
         <v>32.669699999999999</v>
       </c>
-      <c r="J8" s="10">
-        <f t="shared" ref="J8:J10" si="9">I$4/I8</f>
+      <c r="J8" s="7">
+        <f t="shared" ref="J8:J10" si="10">I$4/I8</f>
         <v>16.864862548477642</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="5">
         <v>31.8157</v>
       </c>
-      <c r="L8" s="8">
-        <f t="shared" ref="L8:L10" si="10">K$4/K8</f>
+      <c r="L8" s="5">
+        <f t="shared" ref="L8:L10" si="11">K$4/K8</f>
         <v>18.018525444984711</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="6">
         <v>31.588100000000001</v>
       </c>
-      <c r="N8" s="11">
-        <f t="shared" ref="N8:N9" si="11">M$4/M8</f>
+      <c r="N8" s="8">
+        <f t="shared" ref="N8:N9" si="12">M$4/M8</f>
         <v>17.116034202753568</v>
       </c>
     </row>
@@ -1969,46 +1971,46 @@
       <c r="B9" s="2">
         <v>24</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <v>17.530799999999999</v>
       </c>
-      <c r="D9" s="8">
-        <f>C$4/C9</f>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
         <v>31.39537271544938</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="6">
         <v>17.314</v>
       </c>
-      <c r="F9" s="10">
-        <f t="shared" ref="F9:F10" si="12">E$4/E9</f>
+      <c r="F9" s="7">
+        <f t="shared" ref="F9:F10" si="13">E$4/E9</f>
         <v>32.497285433753035</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="5">
         <v>15.9366</v>
       </c>
-      <c r="H9" s="8">
-        <f t="shared" si="8"/>
+      <c r="H9" s="5">
+        <f t="shared" si="9"/>
         <v>35.326669427606888</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="6">
         <v>16.842400000000001</v>
       </c>
-      <c r="J9" s="10">
-        <f t="shared" si="9"/>
+      <c r="J9" s="7">
+        <f t="shared" si="10"/>
         <v>32.713271267752816</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="5">
         <v>17.427700000000002</v>
       </c>
-      <c r="L9" s="8">
-        <f t="shared" si="10"/>
+      <c r="L9" s="5">
+        <f t="shared" si="11"/>
         <v>32.894300452727556</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="6">
         <v>16.5014</v>
       </c>
-      <c r="N9" s="11">
-        <f t="shared" si="11"/>
+      <c r="N9" s="8">
+        <f t="shared" si="12"/>
         <v>32.764674512465611</v>
       </c>
     </row>
@@ -2016,43 +2018,43 @@
       <c r="B10" s="2">
         <v>32</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>16.600000000000001</v>
       </c>
-      <c r="D10" s="8">
-        <f>C$4/C10</f>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
         <v>33.155783132530118</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="6">
         <v>15.886900000000001</v>
       </c>
-      <c r="F10" s="10">
-        <f t="shared" si="12"/>
+      <c r="F10" s="7">
+        <f t="shared" si="13"/>
         <v>35.416475209134568</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <v>16.595300000000002</v>
       </c>
-      <c r="H10" s="8">
-        <f t="shared" si="8"/>
+      <c r="H10" s="5">
+        <f t="shared" si="9"/>
         <v>33.924484643242359</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="6">
         <v>16.695399999999999</v>
       </c>
-      <c r="J10" s="10">
-        <f t="shared" si="9"/>
+      <c r="J10" s="7">
+        <f t="shared" si="10"/>
         <v>33.001305748888917</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="5">
         <v>16.1953</v>
       </c>
-      <c r="L10" s="8">
-        <f t="shared" si="10"/>
+      <c r="L10" s="5">
+        <f t="shared" si="11"/>
         <v>35.397430118614665</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="11"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="13" spans="2:18">
       <c r="L13" t="s">
@@ -2064,19 +2066,19 @@
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -2085,19 +2087,19 @@
       <c r="K14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="M14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="N14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="12" t="s">
+      <c r="O14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P14" s="12" t="s">
+      <c r="P14" s="9" t="s">
         <v>16</v>
       </c>
       <c r="Q14" s="3" t="s">
@@ -2109,49 +2111,49 @@
       <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="10">
         <v>550.38599999999997</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <v>562.65800000000002</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="10">
         <v>562.98699999999997</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="10">
         <v>550.97</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="10">
         <v>573.27200000000005</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="6">
         <v>540.66300000000001</v>
       </c>
-      <c r="I15" s="11"/>
+      <c r="I15" s="8"/>
       <c r="K15" s="2">
         <v>1</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="10">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="10">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="10">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="10">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="P15" s="13">
+      <c r="P15" s="10">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="Q15" s="6">
         <f>1</f>
         <v>1</v>
       </c>
@@ -2161,50 +2163,50 @@
       <c r="B16" s="2">
         <v>2</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="10">
         <v>267.98500000000001</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="10">
         <v>280.16000000000003</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="10">
         <v>272.84199999999998</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="10">
         <v>271.59300000000002</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="10">
         <v>280.608</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="6">
         <v>271.346</v>
       </c>
-      <c r="I16" s="11"/>
+      <c r="I16" s="8"/>
       <c r="K16" s="2">
         <v>2</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="10">
         <f>C$15/C16</f>
         <v>2.0537940556374421</v>
       </c>
-      <c r="M16" s="13">
-        <f t="shared" ref="M16:Q16" si="13">D$15/D16</f>
+      <c r="M16" s="10">
+        <f t="shared" ref="M16:Q16" si="14">D$15/D16</f>
         <v>2.0083452312964019</v>
       </c>
-      <c r="N16" s="13">
-        <f t="shared" si="13"/>
+      <c r="N16" s="10">
+        <f t="shared" si="14"/>
         <v>2.0634176556395278</v>
       </c>
-      <c r="O16" s="13">
-        <f t="shared" si="13"/>
+      <c r="O16" s="10">
+        <f t="shared" si="14"/>
         <v>2.0286605324879505</v>
       </c>
-      <c r="P16" s="13">
-        <f t="shared" si="13"/>
+      <c r="P16" s="10">
+        <f t="shared" si="14"/>
         <v>2.0429638499258753</v>
       </c>
-      <c r="Q16" s="9">
-        <f t="shared" si="13"/>
+      <c r="Q16" s="6">
+        <f t="shared" si="14"/>
         <v>1.992522462096364</v>
       </c>
       <c r="R16" s="4"/>
@@ -2213,50 +2215,50 @@
       <c r="B17" s="2">
         <v>4</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="10">
         <v>131.54300000000001</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="10">
         <v>133.14500000000001</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="10">
         <v>131.155</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <v>130.91</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="10">
         <v>134.773</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="6">
         <v>136.78399999999999</v>
       </c>
-      <c r="I17" s="11"/>
+      <c r="I17" s="8"/>
       <c r="K17" s="2">
         <v>4</v>
       </c>
-      <c r="L17" s="13">
-        <f t="shared" ref="L17:L21" si="14">C$15/C17</f>
+      <c r="L17" s="10">
+        <f t="shared" ref="L17:L21" si="15">C$15/C17</f>
         <v>4.1840766897516399</v>
       </c>
-      <c r="M17" s="13">
-        <f t="shared" ref="M17:M21" si="15">D$15/D17</f>
+      <c r="M17" s="10">
+        <f t="shared" ref="M17:M21" si="16">D$15/D17</f>
         <v>4.2259040895264564</v>
       </c>
-      <c r="N17" s="13">
-        <f t="shared" ref="N17:N21" si="16">E$15/E17</f>
+      <c r="N17" s="10">
+        <f t="shared" ref="N17:N21" si="17">E$15/E17</f>
         <v>4.292531737257443</v>
       </c>
-      <c r="O17" s="13">
-        <f t="shared" ref="O17:O21" si="17">F$15/F17</f>
+      <c r="O17" s="10">
+        <f t="shared" ref="O17:O21" si="18">F$15/F17</f>
         <v>4.2087693835459481</v>
       </c>
-      <c r="P17" s="13">
-        <f t="shared" ref="P17:P21" si="18">G$15/G17</f>
+      <c r="P17" s="10">
+        <f t="shared" ref="P17:P21" si="19">G$15/G17</f>
         <v>4.2536116284418988</v>
       </c>
-      <c r="Q17" s="9">
-        <f t="shared" ref="Q17:Q21" si="19">H$15/H17</f>
+      <c r="Q17" s="6">
+        <f t="shared" ref="Q17:Q21" si="20">H$15/H17</f>
         <v>3.9526772137092059</v>
       </c>
       <c r="R17" s="4"/>
@@ -2265,50 +2267,50 @@
       <c r="B18" s="2">
         <v>8</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="10">
         <v>66.0471</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="10">
         <v>67.616600000000005</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="10">
         <v>66.313400000000001</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="10">
         <v>65.8596</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="10">
         <v>67.175299999999993</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="6">
         <v>64.299300000000002</v>
       </c>
-      <c r="I18" s="11"/>
+      <c r="I18" s="8"/>
       <c r="K18" s="2">
         <v>8</v>
       </c>
-      <c r="L18" s="13">
-        <f t="shared" si="14"/>
+      <c r="L18" s="10">
+        <f t="shared" si="15"/>
         <v>8.3332349187170962</v>
       </c>
-      <c r="M18" s="13">
-        <f t="shared" si="15"/>
+      <c r="M18" s="10">
+        <f t="shared" si="16"/>
         <v>8.3212997991617446</v>
       </c>
-      <c r="N18" s="13">
-        <f t="shared" si="16"/>
+      <c r="N18" s="10">
+        <f t="shared" si="17"/>
         <v>8.4897924099804865</v>
       </c>
-      <c r="O18" s="13">
-        <f t="shared" si="17"/>
+      <c r="O18" s="10">
+        <f t="shared" si="18"/>
         <v>8.365826698006062</v>
       </c>
-      <c r="P18" s="13">
-        <f t="shared" si="18"/>
+      <c r="P18" s="10">
+        <f t="shared" si="19"/>
         <v>8.5339700753104211</v>
       </c>
-      <c r="Q18" s="9">
-        <f t="shared" si="19"/>
+      <c r="Q18" s="6">
+        <f t="shared" si="20"/>
         <v>8.4085363293224038</v>
       </c>
       <c r="R18" s="4"/>
@@ -2317,50 +2319,50 @@
       <c r="B19" s="2">
         <v>16</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="10">
         <v>32.256</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="10">
         <v>32.5732</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="10">
         <v>32.040500000000002</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="10">
         <v>32.669699999999999</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="10">
         <v>31.8157</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="6">
         <v>31.588100000000001</v>
       </c>
-      <c r="I19" s="11"/>
+      <c r="I19" s="8"/>
       <c r="K19" s="2">
         <v>16</v>
       </c>
-      <c r="L19" s="13">
-        <f t="shared" si="14"/>
+      <c r="L19" s="10">
+        <f t="shared" si="15"/>
         <v>17.063058035714285</v>
       </c>
-      <c r="M19" s="13">
-        <f t="shared" si="15"/>
+      <c r="M19" s="10">
+        <f t="shared" si="16"/>
         <v>17.273648275269242</v>
       </c>
-      <c r="N19" s="13">
-        <f t="shared" si="16"/>
+      <c r="N19" s="10">
+        <f t="shared" si="17"/>
         <v>17.571105319829588</v>
       </c>
-      <c r="O19" s="13">
-        <f t="shared" si="17"/>
+      <c r="O19" s="10">
+        <f t="shared" si="18"/>
         <v>16.864862548477642</v>
       </c>
-      <c r="P19" s="13">
-        <f t="shared" si="18"/>
+      <c r="P19" s="10">
+        <f t="shared" si="19"/>
         <v>18.018525444984711</v>
       </c>
-      <c r="Q19" s="9">
-        <f t="shared" si="19"/>
+      <c r="Q19" s="6">
+        <f t="shared" si="20"/>
         <v>17.116034202753568</v>
       </c>
       <c r="R19" s="4"/>
@@ -2369,50 +2371,50 @@
       <c r="B20" s="2">
         <v>24</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="10">
         <v>17.530799999999999</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="10">
         <v>17.314</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="10">
         <v>15.9366</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="10">
         <v>16.842400000000001</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="10">
         <v>17.427700000000002</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="6">
         <v>16.5014</v>
       </c>
-      <c r="I20" s="11"/>
+      <c r="I20" s="8"/>
       <c r="K20" s="2">
         <v>24</v>
       </c>
-      <c r="L20" s="13">
-        <f t="shared" si="14"/>
+      <c r="L20" s="10">
+        <f t="shared" si="15"/>
         <v>31.39537271544938</v>
       </c>
-      <c r="M20" s="13">
-        <f t="shared" si="15"/>
+      <c r="M20" s="10">
+        <f t="shared" si="16"/>
         <v>32.497285433753035</v>
       </c>
-      <c r="N20" s="13">
-        <f t="shared" si="16"/>
+      <c r="N20" s="10">
+        <f t="shared" si="17"/>
         <v>35.326669427606888</v>
       </c>
-      <c r="O20" s="13">
-        <f t="shared" si="17"/>
+      <c r="O20" s="10">
+        <f t="shared" si="18"/>
         <v>32.713271267752816</v>
       </c>
-      <c r="P20" s="13">
-        <f t="shared" si="18"/>
+      <c r="P20" s="10">
+        <f t="shared" si="19"/>
         <v>32.894300452727556</v>
       </c>
-      <c r="Q20" s="9">
-        <f t="shared" si="19"/>
+      <c r="Q20" s="6">
+        <f t="shared" si="20"/>
         <v>32.764674512465611</v>
       </c>
       <c r="R20" s="4"/>
@@ -2421,47 +2423,52 @@
       <c r="B21" s="2">
         <v>32</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="10">
         <v>16.600000000000001</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="10">
         <v>15.886900000000001</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="10">
         <v>16.595300000000002</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="10">
         <v>16.695399999999999</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="10">
         <v>16.1953</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="11"/>
+      <c r="H21" s="6">
+        <v>19.279800000000002</v>
+      </c>
+      <c r="I21" s="8"/>
       <c r="K21" s="2">
         <v>32</v>
       </c>
-      <c r="L21" s="13">
-        <f t="shared" si="14"/>
+      <c r="L21" s="10">
+        <f t="shared" si="15"/>
         <v>33.155783132530118</v>
       </c>
-      <c r="M21" s="13">
-        <f t="shared" si="15"/>
+      <c r="M21" s="10">
+        <f t="shared" si="16"/>
         <v>35.416475209134568</v>
       </c>
-      <c r="N21" s="13">
-        <f t="shared" si="16"/>
+      <c r="N21" s="10">
+        <f t="shared" si="17"/>
         <v>33.924484643242359</v>
       </c>
-      <c r="O21" s="13">
-        <f t="shared" si="17"/>
+      <c r="O21" s="10">
+        <f t="shared" si="18"/>
         <v>33.001305748888917</v>
       </c>
-      <c r="P21" s="13">
-        <f t="shared" si="18"/>
+      <c r="P21" s="10">
+        <f t="shared" si="19"/>
         <v>35.397430118614665</v>
       </c>
-      <c r="Q21" s="9"/>
+      <c r="Q21" s="6">
+        <f t="shared" si="20"/>
+        <v>28.042977624249211</v>
+      </c>
       <c r="R21" s="4"/>
     </row>
   </sheetData>

</xml_diff>